<commit_message>
shopping list: Add 15V PSU and power jack
</commit_message>
<xml_diff>
--- a/Handleliste-hardware.xlsx
+++ b/Handleliste-hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_7C5055BF84DCCED36523F29B8631F45B3AF06663" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0413299F-91C6-4139-9DAD-E6A95BFD7C2C}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_978B1FBAB96ED5C8A31B68CC47F479601415A1EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4B3F34C-0BAE-446B-8CF2-2653F978FBAF}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,12 +26,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Komponent</t>
   </si>
@@ -115,19 +118,46 @@
   </si>
   <si>
     <t>https://no.mouser.com/ProductDetail/Displaytech/DT043CTFT-IPS-PTS?qs=sGAEpiMZZMt7dcPGmvnkBgpwamjCGwcHY0DbS%252B%2F%2FaodWnRIGq7eMYg%3D%3D</t>
+  </si>
+  <si>
+    <t>OBS! Usikker på om denne passer med PSU. Men vi må ha en tilsvarende komponent</t>
+  </si>
+  <si>
+    <t>15V Power Jack</t>
+  </si>
+  <si>
+    <t>Same Sky</t>
+  </si>
+  <si>
+    <t>PJ-002A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.no/no/products/detail/same-sky-formerly-cui-devices/PJ-002A/96962</t>
+  </si>
+  <si>
+    <t>15V Power Supply</t>
+  </si>
+  <si>
+    <t>Phihong</t>
+  </si>
+  <si>
+    <t>PSA15R-150P6-R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.no/no/products/detail/phihong-usa/PSA15R-150P6-R/5247157</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -135,7 +165,14 @@
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,23 +192,95 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF467886"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -188,10 +297,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -229,150 +338,52 @@
         <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -380,33 +391,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -419,13 +421,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -435,15 +431,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -451,7 +445,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -459,64 +452,39 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G8"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="151" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="151" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="1:7">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -536,7 +504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="1:7" ht="16.350000000000001">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -557,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="1:7" ht="16.350000000000001">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -574,11 +542,11 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G8" si="0">F4*3</f>
+        <f>F4*3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="1:7" ht="16.350000000000001">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -595,11 +563,11 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f>F5*3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="1:7" ht="16.350000000000001">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -616,11 +584,11 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6*3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="1:7" ht="16.350000000000001">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -637,11 +605,11 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7*3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="17.25" customHeight="1">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -658,19 +626,58 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f>F8*3</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{0D2C9F25-4AD3-4082-8BDA-F22BA3FCBCD6}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{4A4C5329-966F-4C9C-B0B8-09550D884900}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{40CC0DE2-AAD9-4680-B86A-B66AE8887CD1}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{FE113CE4-72D6-48A5-B6CE-75F6DEB07DB2}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{F1FCE389-9524-4BCA-B5BD-10DADBD04CE0}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{510D03D2-3255-4DDA-94DC-BA1A7064031C}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{8E7C6E58-EFA3-4A1F-A19D-F161A95142C6}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
handleliste: Add USB-A (?)
Some diff, not sure exactly what it is.
</commit_message>
<xml_diff>
--- a/Handleliste-hardware.xlsx
+++ b/Handleliste-hardware.xlsx
@@ -529,8 +529,8 @@
   </sheetPr>
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: Add LED to handleliste
</commit_message>
<xml_diff>
--- a/Handleliste-hardware.xlsx
+++ b/Handleliste-hardware.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t xml:space="preserve">Komponent</t>
   </si>
@@ -155,14 +155,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.no/no/products/detail/on-shore-technology-inc/USB-A1HSW6/2677750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cree LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JK3030AWT-P-B65EA0000-N0000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.no/no/products/detail/cree-led/JK3030AWT-P-B65EA0000-N0000001/8020361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvisst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motstand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00\ %"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -251,7 +270,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,6 +292,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -527,17 +550,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G12"/>
+  <dimension ref="A2:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="74.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="151"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.71"/>
@@ -761,7 +784,7 @@
       <c r="D12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="6" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="1" t="n">
@@ -770,6 +793,32 @@
       <c r="G12" s="1" t="n">
         <f aca="false">F12*3</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="1" t="e">
+        <f aca="false">F13*3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>